<commit_message>
First Commit PopUa, Triangle and Calendar
</commit_message>
<xml_diff>
--- a/Testing_Calendar.xlsx
+++ b/Testing_Calendar.xlsx
@@ -1368,7 +1368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1384,6 +1384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1584,7 +1590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1593,7 +1599,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1646,6 +1651,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1950,7 +1957,7 @@
   <dimension ref="B2:I480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H206" sqref="H206"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1962,94 +1969,100 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>229</v>
       </c>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="10" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G7" s="19"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="10" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G8" s="20"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="12" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="13" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="12" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="11" t="s">
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="10" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
@@ -2422,12 +2435,12 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2608,12 +2621,12 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>

</xml_diff>